<commit_message>
Generowanie excela, duze zmiany
ja jebie takie gówno cały dzień
</commit_message>
<xml_diff>
--- a/Modele/tescik.xlsx
+++ b/Modele/tescik.xlsx
@@ -149,10 +149,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -566,10 +566,10 @@
           <t>mV</t>
         </is>
       </c>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="3" t="n"/>
-      <c r="F6" s="4" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" s="2" t="n"/>
     </row>
     <row r="7">
       <c r="B7" s="2" t="n">
@@ -581,21 +581,21 @@
       <c r="F7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="5" t="n"/>
+      <c r="B8" s="3" t="n"/>
       <c r="C8" s="2" t="n"/>
       <c r="D8" s="2" t="n"/>
       <c r="E8" s="2" t="n"/>
       <c r="F8" s="2" t="n"/>
     </row>
     <row r="9">
-      <c r="B9" s="5" t="n"/>
+      <c r="B9" s="3" t="n"/>
       <c r="C9" s="2" t="n"/>
       <c r="D9" s="2" t="n"/>
       <c r="E9" s="2" t="n"/>
       <c r="F9" s="2" t="n"/>
     </row>
     <row r="10">
-      <c r="B10" s="6" t="n"/>
+      <c r="B10" s="4" t="n"/>
       <c r="C10" s="2" t="n"/>
       <c r="D10" s="2" t="n"/>
       <c r="E10" s="2" t="n"/>
@@ -607,14 +607,14 @@
           <t>V</t>
         </is>
       </c>
-      <c r="C11" s="3" t="n"/>
-      <c r="D11" s="3" t="n"/>
-      <c r="E11" s="3" t="n"/>
-      <c r="F11" s="4" t="n"/>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="2" t="n"/>
+      <c r="E11" s="2" t="n"/>
+      <c r="F11" s="2" t="n"/>
     </row>
     <row r="12">
       <c r="B12" s="2" t="n">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2" t="n"/>
       <c r="D12" s="2" t="n"/>
@@ -622,21 +622,21 @@
       <c r="F12" s="2" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="5" t="n"/>
+      <c r="B13" s="3" t="n"/>
       <c r="C13" s="2" t="n"/>
       <c r="D13" s="2" t="n"/>
       <c r="E13" s="2" t="n"/>
       <c r="F13" s="2" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" s="5" t="n"/>
+      <c r="B14" s="3" t="n"/>
       <c r="C14" s="2" t="n"/>
       <c r="D14" s="2" t="n"/>
       <c r="E14" s="2" t="n"/>
       <c r="F14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="6" t="n"/>
+      <c r="B15" s="4" t="n"/>
       <c r="C15" s="2" t="n"/>
       <c r="D15" s="2" t="n"/>
       <c r="E15" s="2" t="n"/>
@@ -644,7 +644,7 @@
     </row>
     <row r="16">
       <c r="B16" s="2" t="n">
-        <v>400</v>
+        <v>40</v>
       </c>
       <c r="C16" s="2" t="n"/>
       <c r="D16" s="2" t="n"/>
@@ -652,21 +652,21 @@
       <c r="F16" s="2" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="5" t="n"/>
+      <c r="B17" s="3" t="n"/>
       <c r="C17" s="2" t="n"/>
       <c r="D17" s="2" t="n"/>
       <c r="E17" s="2" t="n"/>
       <c r="F17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="5" t="n"/>
+      <c r="B18" s="3" t="n"/>
       <c r="C18" s="2" t="n"/>
       <c r="D18" s="2" t="n"/>
       <c r="E18" s="2" t="n"/>
       <c r="F18" s="2" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="6" t="n"/>
+      <c r="B19" s="4" t="n"/>
       <c r="C19" s="2" t="n"/>
       <c r="D19" s="2" t="n"/>
       <c r="E19" s="2" t="n"/>
@@ -674,7 +674,7 @@
     </row>
     <row r="20">
       <c r="B20" s="2" t="n">
-        <v>750</v>
+        <v>400</v>
       </c>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="2" t="n"/>
@@ -682,26 +682,56 @@
       <c r="F20" s="2" t="n"/>
     </row>
     <row r="21">
-      <c r="B21" s="5" t="n"/>
+      <c r="B21" s="3" t="n"/>
       <c r="C21" s="2" t="n"/>
       <c r="D21" s="2" t="n"/>
       <c r="E21" s="2" t="n"/>
       <c r="F21" s="2" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="5" t="n"/>
+      <c r="B22" s="3" t="n"/>
       <c r="C22" s="2" t="n"/>
       <c r="D22" s="2" t="n"/>
       <c r="E22" s="2" t="n"/>
       <c r="F22" s="2" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="6" t="n"/>
+      <c r="B23" s="4" t="n"/>
       <c r="C23" s="2" t="n"/>
       <c r="D23" s="2" t="n"/>
       <c r="E23" s="2" t="n"/>
       <c r="F23" s="2" t="n"/>
     </row>
+    <row r="24">
+      <c r="B24" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C24" s="2" t="n"/>
+      <c r="D24" s="2" t="n"/>
+      <c r="E24" s="2" t="n"/>
+      <c r="F24" s="2" t="n"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="3" t="n"/>
+      <c r="C25" s="2" t="n"/>
+      <c r="D25" s="2" t="n"/>
+      <c r="E25" s="2" t="n"/>
+      <c r="F25" s="2" t="n"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="3" t="n"/>
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="n"/>
+      <c r="E26" s="2" t="n"/>
+      <c r="F26" s="2" t="n"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="4" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n"/>
+      <c r="E27" s="2" t="n"/>
+      <c r="F27" s="2" t="n"/>
+    </row>
     <row r="35">
       <c r="B35" s="1" t="inlineStr">
         <is>
@@ -735,10 +765,10 @@
           <t>V</t>
         </is>
       </c>
-      <c r="C36" s="3" t="n"/>
-      <c r="D36" s="3" t="n"/>
-      <c r="E36" s="3" t="n"/>
-      <c r="F36" s="4" t="n"/>
+      <c r="C36" s="2" t="n"/>
+      <c r="D36" s="2" t="n"/>
+      <c r="E36" s="2" t="n"/>
+      <c r="F36" s="2" t="n"/>
     </row>
     <row r="37">
       <c r="B37" s="2" t="n">
@@ -750,21 +780,21 @@
       <c r="F37" s="2" t="n"/>
     </row>
     <row r="38">
-      <c r="B38" s="5" t="n"/>
+      <c r="B38" s="3" t="n"/>
       <c r="C38" s="2" t="n"/>
       <c r="D38" s="2" t="n"/>
       <c r="E38" s="2" t="n"/>
       <c r="F38" s="2" t="n"/>
     </row>
     <row r="39">
-      <c r="B39" s="5" t="n"/>
+      <c r="B39" s="3" t="n"/>
       <c r="C39" s="2" t="n"/>
       <c r="D39" s="2" t="n"/>
       <c r="E39" s="2" t="n"/>
       <c r="F39" s="2" t="n"/>
     </row>
     <row r="40">
-      <c r="B40" s="6" t="n"/>
+      <c r="B40" s="4" t="n"/>
       <c r="C40" s="2" t="n"/>
       <c r="D40" s="2" t="n"/>
       <c r="E40" s="2" t="n"/>
@@ -780,21 +810,21 @@
       <c r="F41" s="2" t="n"/>
     </row>
     <row r="42">
-      <c r="B42" s="5" t="n"/>
+      <c r="B42" s="3" t="n"/>
       <c r="C42" s="2" t="n"/>
       <c r="D42" s="2" t="n"/>
       <c r="E42" s="2" t="n"/>
       <c r="F42" s="2" t="n"/>
     </row>
     <row r="43">
-      <c r="B43" s="5" t="n"/>
+      <c r="B43" s="3" t="n"/>
       <c r="C43" s="2" t="n"/>
       <c r="D43" s="2" t="n"/>
       <c r="E43" s="2" t="n"/>
       <c r="F43" s="2" t="n"/>
     </row>
     <row r="44">
-      <c r="B44" s="6" t="n"/>
+      <c r="B44" s="4" t="n"/>
       <c r="C44" s="2" t="n"/>
       <c r="D44" s="2" t="n"/>
       <c r="E44" s="2" t="n"/>
@@ -833,14 +863,14 @@
           <t>mA</t>
         </is>
       </c>
-      <c r="C66" s="3" t="n"/>
-      <c r="D66" s="3" t="n"/>
-      <c r="E66" s="3" t="n"/>
-      <c r="F66" s="4" t="n"/>
+      <c r="C66" s="2" t="n"/>
+      <c r="D66" s="2" t="n"/>
+      <c r="E66" s="2" t="n"/>
+      <c r="F66" s="2" t="n"/>
     </row>
     <row r="67">
       <c r="B67" s="2" t="n">
-        <v>0.4</v>
+        <v>4</v>
       </c>
       <c r="C67" s="2" t="n"/>
       <c r="D67" s="2" t="n"/>
@@ -848,92 +878,92 @@
       <c r="F67" s="2" t="n"/>
     </row>
     <row r="68">
-      <c r="B68" s="5" t="n"/>
+      <c r="B68" s="3" t="n"/>
       <c r="C68" s="2" t="n"/>
       <c r="D68" s="2" t="n"/>
       <c r="E68" s="2" t="n"/>
       <c r="F68" s="2" t="n"/>
     </row>
     <row r="69">
-      <c r="B69" s="5" t="n"/>
+      <c r="B69" s="3" t="n"/>
       <c r="C69" s="2" t="n"/>
       <c r="D69" s="2" t="n"/>
       <c r="E69" s="2" t="n"/>
       <c r="F69" s="2" t="n"/>
     </row>
     <row r="70">
-      <c r="B70" s="6" t="n"/>
+      <c r="B70" s="4" t="n"/>
       <c r="C70" s="2" t="n"/>
       <c r="D70" s="2" t="n"/>
       <c r="E70" s="2" t="n"/>
       <c r="F70" s="2" t="n"/>
     </row>
     <row r="71">
-      <c r="B71" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C71" s="3" t="n"/>
-      <c r="D71" s="3" t="n"/>
-      <c r="E71" s="3" t="n"/>
-      <c r="F71" s="4" t="n"/>
+      <c r="B71" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="C71" s="2" t="n"/>
+      <c r="D71" s="2" t="n"/>
+      <c r="E71" s="2" t="n"/>
+      <c r="F71" s="2" t="n"/>
     </row>
     <row r="72">
-      <c r="B72" s="2" t="n">
-        <v>0.04</v>
-      </c>
+      <c r="B72" s="3" t="n"/>
       <c r="C72" s="2" t="n"/>
       <c r="D72" s="2" t="n"/>
       <c r="E72" s="2" t="n"/>
       <c r="F72" s="2" t="n"/>
     </row>
     <row r="73">
-      <c r="B73" s="5" t="n"/>
+      <c r="B73" s="3" t="n"/>
       <c r="C73" s="2" t="n"/>
       <c r="D73" s="2" t="n"/>
       <c r="E73" s="2" t="n"/>
       <c r="F73" s="2" t="n"/>
     </row>
     <row r="74">
-      <c r="B74" s="5" t="n"/>
+      <c r="B74" s="4" t="n"/>
       <c r="C74" s="2" t="n"/>
       <c r="D74" s="2" t="n"/>
       <c r="E74" s="2" t="n"/>
       <c r="F74" s="2" t="n"/>
     </row>
     <row r="75">
-      <c r="B75" s="6" t="n"/>
+      <c r="B75" s="2" t="n">
+        <v>400</v>
+      </c>
       <c r="C75" s="2" t="n"/>
       <c r="D75" s="2" t="n"/>
       <c r="E75" s="2" t="n"/>
       <c r="F75" s="2" t="n"/>
     </row>
     <row r="76">
-      <c r="B76" s="2" t="n">
-        <v>0.4</v>
-      </c>
+      <c r="B76" s="3" t="n"/>
       <c r="C76" s="2" t="n"/>
       <c r="D76" s="2" t="n"/>
       <c r="E76" s="2" t="n"/>
       <c r="F76" s="2" t="n"/>
     </row>
     <row r="77">
-      <c r="B77" s="5" t="n"/>
+      <c r="B77" s="3" t="n"/>
       <c r="C77" s="2" t="n"/>
       <c r="D77" s="2" t="n"/>
       <c r="E77" s="2" t="n"/>
       <c r="F77" s="2" t="n"/>
     </row>
     <row r="78">
-      <c r="B78" s="5" t="n"/>
+      <c r="B78" s="4" t="n"/>
       <c r="C78" s="2" t="n"/>
       <c r="D78" s="2" t="n"/>
       <c r="E78" s="2" t="n"/>
       <c r="F78" s="2" t="n"/>
     </row>
     <row r="79">
-      <c r="B79" s="6" t="n"/>
+      <c r="B79" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="C79" s="2" t="n"/>
       <c r="D79" s="2" t="n"/>
       <c r="E79" s="2" t="n"/>
@@ -949,21 +979,21 @@
       <c r="F80" s="2" t="n"/>
     </row>
     <row r="81">
-      <c r="B81" s="5" t="n"/>
+      <c r="B81" s="3" t="n"/>
       <c r="C81" s="2" t="n"/>
       <c r="D81" s="2" t="n"/>
       <c r="E81" s="2" t="n"/>
       <c r="F81" s="2" t="n"/>
     </row>
     <row r="82">
-      <c r="B82" s="5" t="n"/>
+      <c r="B82" s="3" t="n"/>
       <c r="C82" s="2" t="n"/>
       <c r="D82" s="2" t="n"/>
       <c r="E82" s="2" t="n"/>
       <c r="F82" s="2" t="n"/>
     </row>
     <row r="83">
-      <c r="B83" s="6" t="n"/>
+      <c r="B83" s="4" t="n"/>
       <c r="C83" s="2" t="n"/>
       <c r="D83" s="2" t="n"/>
       <c r="E83" s="2" t="n"/>
@@ -1002,14 +1032,14 @@
           <t>mA</t>
         </is>
       </c>
-      <c r="C96" s="3" t="n"/>
-      <c r="D96" s="3" t="n"/>
-      <c r="E96" s="3" t="n"/>
-      <c r="F96" s="4" t="n"/>
+      <c r="C96" s="2" t="n"/>
+      <c r="D96" s="2" t="n"/>
+      <c r="E96" s="2" t="n"/>
+      <c r="F96" s="2" t="n"/>
     </row>
     <row r="97">
       <c r="B97" s="2" t="n">
-        <v>0.004</v>
+        <v>40</v>
       </c>
       <c r="C97" s="2" t="n"/>
       <c r="D97" s="2" t="n"/>
@@ -1017,62 +1047,62 @@
       <c r="F97" s="2" t="n"/>
     </row>
     <row r="98">
-      <c r="B98" s="5" t="n"/>
+      <c r="B98" s="3" t="n"/>
       <c r="C98" s="2" t="n"/>
       <c r="D98" s="2" t="n"/>
       <c r="E98" s="2" t="n"/>
       <c r="F98" s="2" t="n"/>
     </row>
     <row r="99">
-      <c r="B99" s="5" t="n"/>
+      <c r="B99" s="3" t="n"/>
       <c r="C99" s="2" t="n"/>
       <c r="D99" s="2" t="n"/>
       <c r="E99" s="2" t="n"/>
       <c r="F99" s="2" t="n"/>
     </row>
     <row r="100">
-      <c r="B100" s="6" t="n"/>
+      <c r="B100" s="4" t="n"/>
       <c r="C100" s="2" t="n"/>
       <c r="D100" s="2" t="n"/>
       <c r="E100" s="2" t="n"/>
       <c r="F100" s="2" t="n"/>
     </row>
     <row r="101">
-      <c r="B101" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C101" s="3" t="n"/>
-      <c r="D101" s="3" t="n"/>
-      <c r="E101" s="3" t="n"/>
-      <c r="F101" s="4" t="n"/>
+      <c r="B101" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="C101" s="2" t="n"/>
+      <c r="D101" s="2" t="n"/>
+      <c r="E101" s="2" t="n"/>
+      <c r="F101" s="2" t="n"/>
     </row>
     <row r="102">
-      <c r="B102" s="2" t="n">
-        <v>0.4</v>
-      </c>
+      <c r="B102" s="3" t="n"/>
       <c r="C102" s="2" t="n"/>
       <c r="D102" s="2" t="n"/>
       <c r="E102" s="2" t="n"/>
       <c r="F102" s="2" t="n"/>
     </row>
     <row r="103">
-      <c r="B103" s="5" t="n"/>
+      <c r="B103" s="3" t="n"/>
       <c r="C103" s="2" t="n"/>
       <c r="D103" s="2" t="n"/>
       <c r="E103" s="2" t="n"/>
       <c r="F103" s="2" t="n"/>
     </row>
     <row r="104">
-      <c r="B104" s="5" t="n"/>
+      <c r="B104" s="4" t="n"/>
       <c r="C104" s="2" t="n"/>
       <c r="D104" s="2" t="n"/>
       <c r="E104" s="2" t="n"/>
       <c r="F104" s="2" t="n"/>
     </row>
     <row r="105">
-      <c r="B105" s="6" t="n"/>
+      <c r="B105" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="C105" s="2" t="n"/>
       <c r="D105" s="2" t="n"/>
       <c r="E105" s="2" t="n"/>
@@ -1088,21 +1118,21 @@
       <c r="F106" s="2" t="n"/>
     </row>
     <row r="107">
-      <c r="B107" s="5" t="n"/>
+      <c r="B107" s="3" t="n"/>
       <c r="C107" s="2" t="n"/>
       <c r="D107" s="2" t="n"/>
       <c r="E107" s="2" t="n"/>
       <c r="F107" s="2" t="n"/>
     </row>
     <row r="108">
-      <c r="B108" s="5" t="n"/>
+      <c r="B108" s="3" t="n"/>
       <c r="C108" s="2" t="n"/>
       <c r="D108" s="2" t="n"/>
       <c r="E108" s="2" t="n"/>
       <c r="F108" s="2" t="n"/>
     </row>
     <row r="109">
-      <c r="B109" s="6" t="n"/>
+      <c r="B109" s="4" t="n"/>
       <c r="C109" s="2" t="n"/>
       <c r="D109" s="2" t="n"/>
       <c r="E109" s="2" t="n"/>
@@ -1141,14 +1171,14 @@
           <t>Ω</t>
         </is>
       </c>
-      <c r="C126" s="3" t="n"/>
-      <c r="D126" s="3" t="n"/>
-      <c r="E126" s="3" t="n"/>
-      <c r="F126" s="4" t="n"/>
+      <c r="C126" s="5" t="n"/>
+      <c r="D126" s="5" t="n"/>
+      <c r="E126" s="5" t="n"/>
+      <c r="F126" s="6" t="n"/>
     </row>
     <row r="127">
       <c r="B127" s="2" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C127" s="2" t="n"/>
       <c r="D127" s="2" t="n"/>
@@ -1156,7 +1186,7 @@
       <c r="F127" s="2" t="n"/>
     </row>
     <row r="128">
-      <c r="B128" s="6" t="n"/>
+      <c r="B128" s="4" t="n"/>
       <c r="C128" s="2" t="n"/>
       <c r="D128" s="2" t="n"/>
       <c r="E128" s="2" t="n"/>
@@ -1168,10 +1198,10 @@
           <t>kΩ</t>
         </is>
       </c>
-      <c r="C129" s="3" t="n"/>
-      <c r="D129" s="3" t="n"/>
-      <c r="E129" s="3" t="n"/>
-      <c r="F129" s="4" t="n"/>
+      <c r="C129" s="5" t="n"/>
+      <c r="D129" s="5" t="n"/>
+      <c r="E129" s="5" t="n"/>
+      <c r="F129" s="6" t="n"/>
     </row>
     <row r="130">
       <c r="B130" s="2" t="n">
@@ -1183,7 +1213,7 @@
       <c r="F130" s="2" t="n"/>
     </row>
     <row r="131">
-      <c r="B131" s="6" t="n"/>
+      <c r="B131" s="4" t="n"/>
       <c r="C131" s="2" t="n"/>
       <c r="D131" s="2" t="n"/>
       <c r="E131" s="2" t="n"/>
@@ -1191,7 +1221,7 @@
     </row>
     <row r="132">
       <c r="B132" s="2" t="n">
-        <v>200</v>
+        <v>2</v>
       </c>
       <c r="C132" s="2" t="n"/>
       <c r="D132" s="2" t="n"/>
@@ -1199,7 +1229,7 @@
       <c r="F132" s="2" t="n"/>
     </row>
     <row r="133">
-      <c r="B133" s="6" t="n"/>
+      <c r="B133" s="4" t="n"/>
       <c r="C133" s="2" t="n"/>
       <c r="D133" s="2" t="n"/>
       <c r="E133" s="2" t="n"/>
@@ -1207,7 +1237,7 @@
     </row>
     <row r="134">
       <c r="B134" s="2" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C134" s="2" t="n"/>
       <c r="D134" s="2" t="n"/>
@@ -1215,7 +1245,7 @@
       <c r="F134" s="2" t="n"/>
     </row>
     <row r="135">
-      <c r="B135" s="6" t="n"/>
+      <c r="B135" s="4" t="n"/>
       <c r="C135" s="2" t="n"/>
       <c r="D135" s="2" t="n"/>
       <c r="E135" s="2" t="n"/>
@@ -1227,14 +1257,14 @@
           <t>MΩ</t>
         </is>
       </c>
-      <c r="C136" s="3" t="n"/>
-      <c r="D136" s="3" t="n"/>
-      <c r="E136" s="3" t="n"/>
-      <c r="F136" s="4" t="n"/>
+      <c r="C136" s="5" t="n"/>
+      <c r="D136" s="5" t="n"/>
+      <c r="E136" s="5" t="n"/>
+      <c r="F136" s="6" t="n"/>
     </row>
     <row r="137">
       <c r="B137" s="2" t="n">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C137" s="2" t="n"/>
       <c r="D137" s="2" t="n"/>
@@ -1242,7 +1272,7 @@
       <c r="F137" s="2" t="n"/>
     </row>
     <row r="138">
-      <c r="B138" s="6" t="n"/>
+      <c r="B138" s="4" t="n"/>
       <c r="C138" s="2" t="n"/>
       <c r="D138" s="2" t="n"/>
       <c r="E138" s="2" t="n"/>
@@ -1258,7 +1288,9 @@
       <c r="F139" s="2" t="n"/>
     </row>
     <row r="140">
-      <c r="B140" s="6" t="n"/>
+      <c r="B140" s="2" t="n">
+        <v>200</v>
+      </c>
       <c r="C140" s="2" t="n"/>
       <c r="D140" s="2" t="n"/>
       <c r="E140" s="2" t="n"/>
@@ -1269,28 +1301,28 @@
     <mergeCell ref="B126:F126"/>
     <mergeCell ref="B97:B100"/>
     <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B75:B78"/>
     <mergeCell ref="B12:B15"/>
     <mergeCell ref="B130:B131"/>
     <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B71:F71"/>
     <mergeCell ref="B106:B109"/>
-    <mergeCell ref="B102:B105"/>
+    <mergeCell ref="B71:B74"/>
     <mergeCell ref="B96:F96"/>
+    <mergeCell ref="B105:F105"/>
     <mergeCell ref="B67:B70"/>
     <mergeCell ref="B132:B133"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B136:F136"/>
-    <mergeCell ref="B101:F101"/>
+    <mergeCell ref="B101:B104"/>
     <mergeCell ref="B137:B138"/>
     <mergeCell ref="B127:B128"/>
-    <mergeCell ref="B139:B140"/>
     <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B24:B27"/>
     <mergeCell ref="B80:B83"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="B134:B135"/>
-    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B79:F79"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B41:B44"/>

</xml_diff>